<commit_message>
further development of interpolation methods. Code to compare effectiveness of interpolation methods
</commit_message>
<xml_diff>
--- a/fip_collab/2015_09_22_spectral_database_codes/db_truncation_error.xlsx
+++ b/fip_collab/2015_09_22_spectral_database_codes/db_truncation_error.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>retention (%)</t>
   </si>
@@ -39,15 +40,63 @@
   <si>
     <t># frequencies</t>
   </si>
+  <si>
+    <t>percentage of frequencies retained</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">retain frequencies with magnitude &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>% of largest magnitude frequency</t>
+    </r>
+  </si>
+  <si>
+    <t>count of frequencies retained</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -69,13 +118,169 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,11 +551,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156789152"/>
-        <c:axId val="156789544"/>
+        <c:axId val="168992464"/>
+        <c:axId val="168992848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156789152"/>
+        <c:axId val="168992464"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -457,12 +662,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156789544"/>
+        <c:crossAx val="168992848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156789544"/>
+        <c:axId val="168992848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -583,7 +788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156789152"/>
+        <c:crossAx val="168992464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -951,11 +1156,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202475888"/>
-        <c:axId val="202476280"/>
+        <c:axId val="168824896"/>
+        <c:axId val="168072592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202475888"/>
+        <c:axId val="168824896"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1062,12 +1267,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202476280"/>
+        <c:crossAx val="168072592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202476280"/>
+        <c:axId val="168072592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202475888"/>
+        <c:crossAx val="168824896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1572,11 +1777,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202477064"/>
-        <c:axId val="202477456"/>
+        <c:axId val="168822936"/>
+        <c:axId val="168823320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202477064"/>
+        <c:axId val="168822936"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1683,12 +1888,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202477456"/>
+        <c:crossAx val="168823320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202477456"/>
+        <c:axId val="168823320"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1809,7 +2014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202477064"/>
+        <c:crossAx val="168822936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2186,11 +2391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156785232"/>
-        <c:axId val="156783664"/>
+        <c:axId val="168704544"/>
+        <c:axId val="169295256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156785232"/>
+        <c:axId val="168704544"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2311,12 +2516,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156783664"/>
+        <c:crossAx val="169295256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="156783664"/>
+        <c:axId val="169295256"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2437,7 +2642,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156785232"/>
+        <c:crossAx val="168704544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2494,6 +2699,940 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Frequency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> retention vs Database Error</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40098</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250630</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400043</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1061144</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8957952</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.4199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.29E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7600000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2399999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>5.6469999999999997E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="253659776"/>
+        <c:axId val="253659384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="253659776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>number of frequencies</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> retained</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="253659384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="253659384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>error in plastic strain prediction (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="253659776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Frequency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> retention vs Database Error</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$13:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5597</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41888</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>262594</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>427022</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1228527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11520000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$13:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.43E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6399999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8400000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>5.0820000000000001E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="253661344"/>
+        <c:axId val="414934424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="253661344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>number of frequencies</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> retained</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414934424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="414934424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>error in plastic strain prediction (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="253661344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2657,6 +3796,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4206,6 +5425,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4847,6 +7098,68 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38102</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>133352</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5139,8 +7452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5459,4 +7772,200 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D9:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="9" max="11" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="4:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>405</v>
+      </c>
+      <c r="K11" s="6">
+        <v>4.5199999999999997E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5399</v>
+      </c>
+      <c r="K12" s="2">
+        <v>6.0299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J13" s="2">
+        <v>40098</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>250630</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2.798</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="J15" s="2">
+        <v>400043</v>
+      </c>
+      <c r="K15" s="2">
+        <v>4.4660000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1061144</v>
+      </c>
+      <c r="K16" s="2">
+        <v>11.846</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>8957952</v>
+      </c>
+      <c r="K17" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I19" s="6">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6">
+        <v>433</v>
+      </c>
+      <c r="K19" s="6">
+        <v>6.2600000000000004E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5597</v>
+      </c>
+      <c r="K20" s="2">
+        <v>8.0999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J21" s="2">
+        <v>41888</v>
+      </c>
+      <c r="K21" s="2">
+        <v>6.0600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="J22" s="2">
+        <v>262594</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I23" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="J23" s="2">
+        <v>427022</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.61799999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1228527</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1.7769999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>11520000</v>
+      </c>
+      <c r="K25" s="3">
+        <v>16.667000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>